<commit_message>
beginning of processed file removal. Requires 'iterate' mechanism refactorring
</commit_message>
<xml_diff>
--- a/Squanched/TODO.xlsx
+++ b/Squanched/TODO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="1425" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>4) ניהול מקום (מחיקת קבצים תוך כדי ריצה)</t>
-  </si>
-  <si>
-    <t>5) צמצום שימוש בCPU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>6) BACKUP CORRUPTION</t>
   </si>
@@ -37,9 +31,6 @@
     <t>10) לעטוף את DEC ואת ENC לקובץ אחד</t>
   </si>
   <si>
-    <t>11) CLEANUP</t>
-  </si>
-  <si>
     <t>12) WORD  הנדסת אנוש</t>
   </si>
   <si>
@@ -62,17 +53,23 @@
   </si>
   <si>
     <t>לנסות לדבר שוב עם השרת</t>
+  </si>
+  <si>
+    <t>גילוי קבצים מוצפנים בסיום הריצה</t>
+  </si>
+  <si>
+    <t>רפקטורינג למנגנון iterate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -195,6 +192,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -230,6 +244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,95 +437,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B18"/>
+  <dimension ref="B3:B20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO update. Adress the first block first!
</commit_message>
<xml_diff>
--- a/Squanched/TODO.xlsx
+++ b/Squanched/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>6) BACKUP CORRUPTION</t>
   </si>
@@ -22,9 +22,6 @@
     <t>8) OVERALL TEST על מכונה וירטואלית</t>
   </si>
   <si>
-    <t>9) זכרון</t>
-  </si>
-  <si>
     <t>10) לעטוף את DEC ואת ENC לקובץ אחד</t>
   </si>
   <si>
@@ -55,7 +52,22 @@
     <t>רפקטורינג למנגנון iterate</t>
   </si>
   <si>
-    <t>7) הודעה ללקוח -  restart וביטול רישום ל-startup processes</t>
+    <t>rsa-based head-of-file encryption</t>
+  </si>
+  <si>
+    <t>7) הודעה ללקוח -  ביטול רישום ל-startup processes</t>
+  </si>
+  <si>
+    <t>כמה אנטיוירוסים</t>
+  </si>
+  <si>
+    <t>בדיקת stratup</t>
+  </si>
+  <si>
+    <t>בדיקת מאקרו</t>
+  </si>
+  <si>
+    <t>מיפוי כוננים נוספים - כולל USB DRIVES</t>
   </si>
 </sst>
 </file>
@@ -434,96 +446,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C20"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix for bug in lnk files iteration
iterate was called with lnk files directly, even if they were not
targeting directories. Caused crash, fixed with a query.

Also, template macro doesn't ask for administrator privilages for exe
</commit_message>
<xml_diff>
--- a/Squanched/TODO.xlsx
+++ b/Squanched/TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="1425" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>6) BACKUP CORRUPTION</t>
   </si>
@@ -22,21 +22,12 @@
     <t>8) OVERALL TEST על מכונה וירטואלית</t>
   </si>
   <si>
-    <t>10) לעטוף את DEC ואת ENC לקובץ אחד</t>
-  </si>
-  <si>
     <t>12) WORD  הנדסת אנוש</t>
   </si>
   <si>
     <t>13) סיומת קובץ 5 תווים אקריים/ קבצי PDF עם MAGIC</t>
   </si>
   <si>
-    <t>14) להמנע מקבצים מוסתרים</t>
-  </si>
-  <si>
-    <t>15) חזרה בRESTART</t>
-  </si>
-  <si>
     <t>16) מיון קבצים נוסף לפי גודל</t>
   </si>
   <si>
@@ -46,15 +37,6 @@
     <t>לסגור ווינדוס דפנדר</t>
   </si>
   <si>
-    <t>גילוי קבצים מוצפנים בסיום הריצה</t>
-  </si>
-  <si>
-    <t>רפקטורינג למנגנון iterate</t>
-  </si>
-  <si>
-    <t>rsa-based head-of-file encryption</t>
-  </si>
-  <si>
     <t>7) הודעה ללקוח -  ביטול רישום ל-startup processes</t>
   </si>
   <si>
@@ -67,7 +49,10 @@
     <t>בדיקת מאקרו</t>
   </si>
   <si>
-    <t>מיפוי כוננים נוספים - כולל USB DRIVES</t>
+    <t>להוסיף קריאה לbatch file.</t>
+  </si>
+  <si>
+    <t>הצפנה חלקית</t>
   </si>
 </sst>
 </file>
@@ -446,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,12 +446,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>12</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -476,72 +464,54 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>13</v>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>